<commit_message>
Cerrando la solucion v1
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A1147C2-75EF-467F-ACA7-198BFFE1A726}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF9D744-A6AF-43FA-872D-96A0FEAD3FEC}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2250" yWindow="975" windowWidth="15675" windowHeight="9945" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>P</t>
-  </si>
-  <si>
-    <t>FLAG_Account</t>
   </si>
   <si>
     <t>S</t>
@@ -148,13 +145,75 @@
   <si>
     <t>TARJETA 
 DE CREDITO</t>
+  </si>
+  <si>
+    <t>current_amount</t>
+  </si>
+  <si>
+    <t>starting_amount</t>
+  </si>
+  <si>
+    <t>flag_account</t>
+  </si>
+  <si>
+    <t>quota</t>
+  </si>
+  <si>
+    <t>IdBANKCARD</t>
+  </si>
+  <si>
+    <t>IdAccountCustomer</t>
+  </si>
+  <si>
+    <t>IdCustomer</t>
+  </si>
+  <si>
+    <t>fecha inicio</t>
+  </si>
+  <si>
+    <t>fecha pago</t>
+  </si>
+  <si>
+    <t>paymentdate</t>
+  </si>
+  <si>
+    <t>startdate</t>
+  </si>
+  <si>
+    <t>fecha de corte</t>
+  </si>
+  <si>
+    <t>courtdate</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TARJETA DE CREDITO</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>TARJETA DEBITO</t>
+  </si>
+  <si>
+    <t>FLAG_Account
+(P:PRINCIAL;
+S:SECUNDARIA)</t>
+  </si>
+  <si>
+    <t>FLAG_CREATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,16 +221,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -259,26 +354,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,364 +801,530 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5674F0F-6139-4E44-BB13-7234BF3ED0EA}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="11" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="20.42578125" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="P2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1200</v>
+      </c>
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7">
+        <v>1400</v>
+      </c>
+      <c r="N4" s="7">
+        <v>10</v>
+      </c>
+      <c r="O4" s="7">
+        <v>7000</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="6">
+        <v>2</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1400</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7">
+        <v>7000</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="6"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="9"/>
+    </row>
+    <row r="6" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>700</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>700</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="T7" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" s="25"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="9" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="8"/>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M13" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="N13" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M14" s="4">
         <v>1</v>
       </c>
-      <c r="L2" s="6">
-        <v>50</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>8</v>
+      <c r="N14" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="5">
-        <v>1</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1200</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9">
-        <v>1400</v>
-      </c>
-      <c r="M4" s="9">
-        <v>10</v>
-      </c>
-      <c r="N4" s="9">
-        <v>7000</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="8">
-        <v>2</v>
-      </c>
-      <c r="L5" s="9">
-        <v>1400</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9">
-        <v>7000</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
-        <v>700</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>700</v>
-      </c>
-      <c r="C7" s="6">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L10" s="5">
-        <v>1</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L11" s="5">
-        <v>1</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L12" s="8">
-        <v>2</v>
-      </c>
-      <c r="M12" s="12" t="s">
+      <c r="N15" s="29" t="s">
         <v>27</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando info tabla customer
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtorrrom\Documents\QUARKUS\BOOTCAMP\git\tarea1\designsolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF9D744-A6AF-43FA-872D-96A0FEAD3FEC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6E452B-F00C-4599-A7E1-06888A390D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -207,6 +207,39 @@
   </si>
   <si>
     <t>FLAG_CREATION</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>idCustomer</t>
+  </si>
+  <si>
+    <t>typeCustomer</t>
+  </si>
+  <si>
+    <t>numberDocument</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>JUAN</t>
+  </si>
+  <si>
+    <t>TORRES ROMERO</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>COMPANY SAC</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -449,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -464,7 +497,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,12 +505,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -801,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5674F0F-6139-4E44-BB13-7234BF3ED0EA}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,40 +882,40 @@
       <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -912,7 +941,6 @@
       <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="21"/>
       <c r="K2" t="s">
         <v>28</v>
       </c>
@@ -954,7 +982,6 @@
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="21"/>
       <c r="K3" t="s">
         <v>29</v>
       </c>
@@ -971,7 +998,6 @@
         <v>8</v>
       </c>
       <c r="R3" s="4"/>
-      <c r="S3" s="21"/>
       <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1018,7 +1044,6 @@
         <v>8</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="21"/>
       <c r="T4" s="5"/>
     </row>
     <row r="5" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1095,7 +1120,7 @@
       <c r="I6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="26" t="s">
         <v>55</v>
       </c>
       <c r="K6" s="11" t="s">
@@ -1156,27 +1181,27 @@
         <v>49</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22" t="s">
+      <c r="N7" s="18"/>
+      <c r="O7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" s="22" t="s">
+      <c r="Q7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22" t="s">
+      <c r="R7" s="18"/>
+      <c r="S7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="T7" s="19" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1203,33 +1228,32 @@
         <v>24</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="12" t="s">
+      <c r="J8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24" t="s">
+      <c r="L8" s="20"/>
+      <c r="M8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="R8" s="24" t="s">
+      <c r="R8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="T8" s="25"/>
+      <c r="T8" s="21"/>
     </row>
     <row r="9" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
@@ -1257,19 +1281,19 @@
       <c r="J9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="22" t="s">
         <v>52</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-      <c r="P9" s="26" t="s">
+      <c r="P9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Q9" s="26" t="s">
+      <c r="Q9" s="22" t="s">
         <v>52</v>
       </c>
       <c r="R9" s="7"/>
@@ -1278,10 +1302,10 @@
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M12" s="14" t="s">
+      <c r="M12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="N12" s="23" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1289,13 +1313,13 @@
       <c r="M13" s="4">
         <v>1</v>
       </c>
-      <c r="N13" s="28" t="s">
+      <c r="N13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="12" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1303,13 +1327,13 @@
       <c r="M14" s="4">
         <v>1</v>
       </c>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="13" t="s">
+      <c r="P14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" s="13" t="s">
+      <c r="Q14" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1317,14 +1341,70 @@
       <c r="M15" s="6">
         <v>2</v>
       </c>
-      <c r="N15" s="29" t="s">
+      <c r="N15" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="Q15" s="13" t="s">
+      <c r="Q15" s="12" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="9:13" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20">
+        <v>44556655</v>
+      </c>
+      <c r="L20" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21">
+        <v>12345678989</v>
+      </c>
+      <c r="L21" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cerrando la solucion v2
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF9D744-A6AF-43FA-872D-96A0FEAD3FEC}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3F30A18-2195-4467-9AA7-0162DA7B5E00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -207,6 +207,14 @@
   </si>
   <si>
     <t>FLAG_CREATION</t>
+  </si>
+  <si>
+    <t>estado
+(A:activo;
+I:Inactivo)</t>
+  </si>
+  <si>
+    <t>state</t>
   </si>
 </sst>
 </file>
@@ -449,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -464,7 +472,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,12 +480,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -487,6 +491,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5674F0F-6139-4E44-BB13-7234BF3ED0EA}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J7" sqref="J7:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +846,7 @@
     <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,44 +868,47 @@
       <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="17" t="s">
         <v>47</v>
       </c>
+      <c r="U1" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -912,7 +930,6 @@
       <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="21"/>
       <c r="K2" t="s">
         <v>28</v>
       </c>
@@ -932,7 +949,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -954,7 +971,6 @@
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="21"/>
       <c r="K3" t="s">
         <v>29</v>
       </c>
@@ -971,10 +987,9 @@
         <v>8</v>
       </c>
       <c r="R3" s="4"/>
-      <c r="S3" s="21"/>
       <c r="T3" s="5"/>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1018,10 +1033,9 @@
         <v>8</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="21"/>
       <c r="T4" s="5"/>
     </row>
-    <row r="5" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1070,7 +1084,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1095,7 +1109,7 @@
       <c r="I6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="26" t="s">
         <v>55</v>
       </c>
       <c r="K6" s="11" t="s">
@@ -1128,8 +1142,11 @@
       <c r="T6" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="U6" s="28" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1152,35 +1169,38 @@
         <v>18</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="34" t="s">
         <v>49</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22" t="s">
+      <c r="N7" s="18"/>
+      <c r="O7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" s="22" t="s">
+      <c r="Q7" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22" t="s">
+      <c r="R7" s="18"/>
+      <c r="S7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="T7" s="19" t="s">
         <v>49</v>
       </c>
+      <c r="U7" s="32" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1203,35 +1223,37 @@
         <v>24</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24" t="s">
+      <c r="L8" s="20"/>
+      <c r="M8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="R8" s="24" t="s">
+      <c r="R8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="T8" s="25"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="32" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1254,76 +1276,79 @@
         <v>24</v>
       </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="22" t="s">
         <v>52</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
-      <c r="P9" s="26" t="s">
+      <c r="P9" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="Q9" s="26" t="s">
+      <c r="Q9" s="31" t="s">
         <v>52</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="8"/>
+      <c r="U9" s="33" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M12" s="14" t="s">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="N12" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M13" s="4">
         <v>1</v>
       </c>
-      <c r="N13" s="28" t="s">
+      <c r="N13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="M14" s="4">
         <v>1</v>
       </c>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="13" t="s">
+      <c r="P14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" s="13" t="s">
+      <c r="Q14" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M15" s="6">
         <v>2</v>
       </c>
-      <c r="N15" s="29" t="s">
+      <c r="N15" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="Q15" s="13" t="s">
+      <c r="Q15" s="12" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cerrando la solucion v4
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75DCFDCC-076D-4161-AE70-99D33D9C18A5}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26F57899-F4C1-465E-9C5E-EEC359325229}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
+    <workbookView minimized="1" xWindow="2940" yWindow="975" windowWidth="15675" windowHeight="9945" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -851,32 +851,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5674F0F-6139-4E44-BB13-7234BF3ED0EA}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1029,9 +1030,6 @@
       <c r="B4">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -1124,9 +1122,6 @@
       <c r="B6">
         <v>700</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
@@ -1239,9 +1234,6 @@
       </c>
       <c r="B8">
         <v>15</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -1351,6 +1343,12 @@
       <c r="L12" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="N12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H13" s="4">
@@ -1368,11 +1366,11 @@
       <c r="L13">
         <v>45</v>
       </c>
-      <c r="P13" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q13" s="12" t="s">
-        <v>49</v>
+      <c r="N13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1391,11 +1389,11 @@
       <c r="L14">
         <v>324</v>
       </c>
-      <c r="P14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q14" s="12" t="s">
-        <v>14</v>
+      <c r="N14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1413,12 +1411,6 @@
       </c>
       <c r="L15">
         <v>342</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q15" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Semana 02- mejorando el requerimiento
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26F57899-F4C1-465E-9C5E-EEC359325229}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="8_{9AA205DA-BE4E-4AA8-9677-FDF646508860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6D9F12B-C557-48FF-A760-57EB507F9244}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2940" yWindow="975" windowWidth="15675" windowHeight="9945" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20ED7F64-77E5-4C63-8A27-C10C553B1044}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
   <si>
     <t>id</t>
   </si>
@@ -59,9 +59,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>USUARIO</t>
-  </si>
-  <si>
     <t>LOPEZ</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>AHORRO</t>
   </si>
   <si>
-    <t>SUELDO</t>
-  </si>
-  <si>
     <t>idoperationorigin</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
   </si>
   <si>
     <t>cuota</t>
-  </si>
-  <si>
-    <t>004lopez</t>
   </si>
   <si>
     <t>TARJETA 
@@ -260,6 +251,55 @@
   </si>
   <si>
     <t>12/02/2024</t>
+  </si>
+  <si>
+    <t>idaccountcustomer
+(id de la tabla)</t>
+  </si>
+  <si>
+    <t>0000003</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>CUENTA BANCARIA</t>
+  </si>
+  <si>
+    <t>005lopez</t>
+  </si>
+  <si>
+    <t>MILLONARIO</t>
+  </si>
+  <si>
+    <t>DANTE</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ACCOUNTNUMBER</t>
+  </si>
+  <si>
+    <t>accountnumber</t>
+  </si>
+  <si>
+    <t>006lopez</t>
+  </si>
+  <si>
+    <t>007lopez</t>
+  </si>
+  <si>
+    <t>TARJETA DE DEBITO</t>
+  </si>
+  <si>
+    <t>IDTARJETA(FK)</t>
+  </si>
+  <si>
+    <t>USUARIO (FK)</t>
+  </si>
+  <si>
+    <t>IDACCOUNTORIGINI</t>
   </si>
 </sst>
 </file>
@@ -299,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,8 +358,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -483,11 +535,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -531,6 +596,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5674F0F-6139-4E44-BB13-7234BF3ED0EA}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,22 +945,24 @@
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,61 +970,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>7</v>
-      </c>
       <c r="R1" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W1" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -959,31 +1047,44 @@
         <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="4">
+      <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J2" s="43">
+        <v>561651651</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="37">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="3"/>
+      <c r="W2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1000,473 +1101,647 @@
         <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="4">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="44"/>
+      <c r="K3" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="4">
         <v>1</v>
       </c>
-      <c r="M3">
-        <v>1200</v>
-      </c>
-      <c r="P3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="4"/>
-      <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="V3" s="5"/>
+      <c r="W3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="J4" s="44">
+        <v>234234243</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="V4" s="5"/>
+      <c r="W4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7">
-        <v>1400</v>
-      </c>
-      <c r="N4" s="7">
-        <v>10</v>
-      </c>
-      <c r="O4" s="7">
-        <v>7000</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="4"/>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4</v>
+      </c>
+      <c r="J5" s="45">
+        <v>654651</v>
+      </c>
       <c r="K5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="6">
+        <v>47</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7">
+        <v>1400</v>
+      </c>
+      <c r="P5" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>7000</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5</v>
+      </c>
+      <c r="J6" s="45">
+        <v>23561651</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7">
+        <v>1</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="T6" s="4"/>
+      <c r="V6" s="5"/>
+      <c r="W6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="4">
+        <v>6</v>
+      </c>
+      <c r="J7" s="45"/>
+      <c r="K7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="6">
         <v>2</v>
       </c>
-      <c r="M5" s="7">
+      <c r="O7" s="7">
         <v>1400</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7">
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7">
         <v>7000</v>
       </c>
-      <c r="P5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="9"/>
-    </row>
-    <row r="6" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>700</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="R7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="9"/>
+      <c r="W7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="U6" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>700</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q7" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="T7" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="U7" s="29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>7</v>
       </c>
       <c r="B8">
         <v>15</v>
       </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
       <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>700</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="W9" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>700</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="S10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="V10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W10" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="T11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="U11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="V11" s="21"/>
+      <c r="W11" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7">
+        <v>15</v>
+      </c>
+      <c r="C12" s="7">
+        <v>7</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="J16" s="39"/>
+      <c r="K16">
+        <v>23</v>
+      </c>
+      <c r="L16" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="M16" s="34"/>
+      <c r="N16">
+        <v>45</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="P8" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="R8" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="S8" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="T8" s="21"/>
-      <c r="U8" s="29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7">
-        <v>15</v>
-      </c>
-      <c r="C9" s="7">
-        <v>7</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q9" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:21" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="11" t="s">
+      <c r="J17" s="39"/>
+      <c r="K17">
+        <v>53</v>
+      </c>
+      <c r="L17" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" s="11" t="s">
+      <c r="M17" s="34"/>
+      <c r="N17">
+        <v>324</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="8:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="6">
+        <v>3</v>
+      </c>
+      <c r="I18" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="N12" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H13" s="4">
+      <c r="J18" s="39"/>
+      <c r="K18">
+        <v>34</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="34"/>
+      <c r="N18">
+        <v>342</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="8:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H22" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H23">
         <v>1</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I23" t="s">
         <v>25</v>
       </c>
-      <c r="J13">
-        <v>23</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="L13">
-        <v>45</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H14" s="4">
-        <v>1</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14">
-        <v>53</v>
-      </c>
-      <c r="K14" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14">
-        <v>324</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H15" s="6">
+      <c r="K23">
+        <v>44556655</v>
+      </c>
+      <c r="L23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H24">
         <v>2</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="L15">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="8:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L19" s="11" t="s">
+      <c r="I24" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20">
-        <v>44556655</v>
-      </c>
-      <c r="K20" t="s">
+      <c r="K24">
+        <v>12345678989</v>
+      </c>
+      <c r="L24" t="s">
         <v>63</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N24" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21">
-        <v>12345678989</v>
-      </c>
-      <c r="K21" t="s">
-        <v>66</v>
-      </c>
-      <c r="L21" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solution of proyect 2
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AARICOCH\Documents\Bootcamp\AppBancoQuarkus\designsolution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="98" documentId="11_409317D2FE7A9FD1140F4D701475DD773704CC54" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4D5E52-250D-407D-BAE8-4DCCA45BE83C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="126">
   <si>
     <t>id</t>
   </si>
@@ -311,12 +301,120 @@
   </si>
   <si>
     <t>deuda atrasada</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NRO TARJETA</t>
+  </si>
+  <si>
+    <t>REQUEST</t>
+  </si>
+  <si>
+    <t>FECHA DE VENCIMIENTO</t>
+  </si>
+  <si>
+    <t>CODIGO VALIDACION</t>
+  </si>
+  <si>
+    <t>RESPONSE</t>
+  </si>
+  <si>
+    <t>FLAG_AUTORIZACION</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>NRO DOCUMENTO</t>
+  </si>
+  <si>
+    <t>DATOS CLIENTE</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>CREAR</t>
+  </si>
+  <si>
+    <t>MODIFICAR</t>
+  </si>
+  <si>
+    <t>CLAVE(6 DIGITOS)</t>
+  </si>
+  <si>
+    <t>REGISTRO MULTICANAL</t>
+  </si>
+  <si>
+    <t>VALIDATION MULTICANAL</t>
+  </si>
+  <si>
+    <t>VERIFICAR QUE NO SE REPITA NO REGISTRE DOS TD EN EL CLIENTE</t>
+  </si>
+  <si>
+    <t>NRO TARJETA DE DEBITO</t>
+  </si>
+  <si>
+    <t>CONSULTA MICROSERVICIOS</t>
+  </si>
+  <si>
+    <t>CONSULTA DE CUENTAS - SALDOS Y PRODUCTO POR CLIENTE</t>
+  </si>
+  <si>
+    <t>CONSULTA DE OPERACIONES - CUENTA BANCARIA</t>
+  </si>
+  <si>
+    <t>CONSULTA DE OPERACIONES - TARJETA DE CREDITO</t>
+  </si>
+  <si>
+    <t>CONSULTA DE OPERACIONES -  CREDITO</t>
+  </si>
+  <si>
+    <t>AUDITORIA</t>
+  </si>
+  <si>
+    <t>MSAUDITORIA</t>
+  </si>
+  <si>
+    <t>tabla user</t>
+  </si>
+  <si>
+    <t>MONGO</t>
+  </si>
+  <si>
+    <t>FLAG</t>
+  </si>
+  <si>
+    <t>DATOS TARJETA</t>
+  </si>
+  <si>
+    <t>RESPONDER</t>
+  </si>
+  <si>
+    <t>TRUE O FALSE</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>tabla AUDITORIA</t>
+  </si>
+  <si>
+    <t>CODE_CLIENTE</t>
+  </si>
+  <si>
+    <t>CODE_TARJETA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,7 +448,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,8 +479,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -559,11 +663,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -611,10 +730,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -622,8 +738,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,10 +772,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,42 +1070,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.109375" customWidth="1"/>
-    <col min="11" max="11" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.109375" customWidth="1"/>
-    <col min="24" max="24" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1129,7 @@
       <c r="I1" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="39" t="s">
         <v>78</v>
       </c>
       <c r="K1" s="25" t="s">
@@ -1040,14 +1168,14 @@
       <c r="V1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="46" t="s">
+      <c r="W1" s="43" t="s">
         <v>89</v>
       </c>
       <c r="X1" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1072,16 +1200,16 @@
       <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="40">
         <v>561651651</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="37">
+      <c r="M2">
         <v>2</v>
       </c>
       <c r="N2" s="4"/>
@@ -1097,12 +1225,11 @@
       <c r="T2" s="1"/>
       <c r="U2" s="2"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="38"/>
       <c r="X2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1125,8 +1252,8 @@
       <c r="I3" s="4">
         <v>2</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="37" t="s">
+      <c r="J3" s="41"/>
+      <c r="K3" t="s">
         <v>48</v>
       </c>
       <c r="N3" s="4">
@@ -1143,22 +1270,21 @@
       </c>
       <c r="T3" s="4"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="38"/>
       <c r="X3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="41">
         <v>234234243</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" t="s">
         <v>72</v>
       </c>
       <c r="L4" t="s">
@@ -1179,12 +1305,11 @@
       </c>
       <c r="T4" s="4"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="38"/>
       <c r="X4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1209,7 +1334,7 @@
       <c r="I5" s="4">
         <v>4</v>
       </c>
-      <c r="J5" s="45">
+      <c r="J5" s="42">
         <v>654651</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1235,9 +1360,8 @@
       </c>
       <c r="T5" s="4"/>
       <c r="V5" s="5"/>
-      <c r="W5" s="38"/>
-    </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6" t="s">
@@ -1246,7 +1370,7 @@
       <c r="I6" s="4">
         <v>5</v>
       </c>
-      <c r="J6" s="45">
+      <c r="J6" s="42">
         <v>23561651</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -1270,12 +1394,11 @@
       </c>
       <c r="T6" s="4"/>
       <c r="V6" s="5"/>
-      <c r="W6" s="38"/>
       <c r="X6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
@@ -1284,7 +1407,7 @@
       <c r="I7" s="4">
         <v>6</v>
       </c>
-      <c r="J7" s="45"/>
+      <c r="J7" s="42"/>
       <c r="K7" s="7" t="s">
         <v>45</v>
       </c>
@@ -1309,12 +1432,12 @@
       <c r="T7" s="6"/>
       <c r="U7" s="7"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="39"/>
+      <c r="W7" s="34"/>
       <c r="X7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -1340,7 +1463,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -1362,7 +1485,7 @@
       <c r="I9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="38" t="s">
         <v>79</v>
       </c>
       <c r="K9" s="25" t="s">
@@ -1404,7 +1527,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -1456,12 +1579,12 @@
       <c r="V10" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="W10" s="47"/>
+      <c r="W10" s="20"/>
       <c r="X10" s="29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -1481,7 +1604,6 @@
         <v>22</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="38"/>
       <c r="K11" s="31" t="s">
         <v>47</v>
       </c>
@@ -1508,12 +1630,12 @@
         <v>47</v>
       </c>
       <c r="V11" s="21"/>
-      <c r="W11" s="47"/>
+      <c r="W11" s="20"/>
       <c r="X11" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>8</v>
       </c>
@@ -1559,12 +1681,11 @@
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="8"/>
-      <c r="W12" s="38"/>
       <c r="X12" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -1583,14 +1704,14 @@
       <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="37" t="s">
         <v>72</v>
       </c>
       <c r="L13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -1613,7 +1734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H15" s="13" t="s">
         <v>27</v>
       </c>
@@ -1641,7 +1762,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -1663,7 +1784,7 @@
       <c r="I16" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="39"/>
+      <c r="J16" s="34"/>
       <c r="K16">
         <v>23</v>
       </c>
@@ -1684,7 +1805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1709,7 +1830,7 @@
       <c r="I17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="39"/>
+      <c r="J17" s="34"/>
       <c r="K17">
         <v>53</v>
       </c>
@@ -1730,7 +1851,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1758,7 +1879,7 @@
       <c r="I18" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="J18" s="39"/>
+      <c r="J18" s="34"/>
       <c r="K18">
         <v>34</v>
       </c>
@@ -1779,12 +1900,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="24" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:17" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H22" s="11" t="s">
         <v>55</v>
       </c>
@@ -1803,7 +1924,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H23">
         <v>1</v>
       </c>
@@ -1820,13 +1941,22 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H24">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2">
         <v>2</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="J24" s="3"/>
       <c r="K24">
         <v>12345678989</v>
       </c>
@@ -1837,7 +1967,292 @@
         <v>64</v>
       </c>
     </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="51"/>
+      <c r="C25" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="51"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" t="s">
+        <v>100</v>
+      </c>
+      <c r="J26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="51"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>122</v>
+      </c>
+      <c r="J27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="51"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="51"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="51"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="51"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="51"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="51"/>
+      <c r="C33" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="51"/>
+      <c r="C34" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I34" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="51"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="51"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="51"/>
+      <c r="C37" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="51"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="51"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="51"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="51"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="52"/>
+      <c r="C42" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C43" s="55" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B24:B42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ordenando la solution v1
</commit_message>
<xml_diff>
--- a/SIMULATION-DATA.xlsx
+++ b/SIMULATION-DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/acespedc_emeal_nttdata_com/Documents/Escritorio/QUARKUS/PROYECTO/PRIMER SEMANA/designsolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="11_409317D2FE7A9FD1140F4D701475DD773704CC54" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67C7045C-84E0-46DE-AF90-EAAC3F6E7FBC}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="11_409317D2FE7A9FD1140F4D701475DD773704CC54" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C285DFD-99EA-42E4-B7FF-B81B855CB0E5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -766,6 +766,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,16 +784,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,7 +1101,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1127,7 @@
     <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" style="56" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" style="52" customWidth="1"/>
     <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1196,7 +1195,7 @@
       <c r="V1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="54" t="s">
+      <c r="W1" s="51" t="s">
         <v>86</v>
       </c>
       <c r="X1" s="26" t="s">
@@ -1228,7 +1227,7 @@
       <c r="I2" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="56" t="s">
         <v>125</v>
       </c>
       <c r="K2" t="s">
@@ -1256,7 +1255,7 @@
       <c r="S2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="51">
+      <c r="T2" s="48">
         <v>44979</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -1265,7 +1264,7 @@
       <c r="V2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="W2" s="55" t="s">
+      <c r="W2" s="52" t="s">
         <v>123</v>
       </c>
       <c r="X2" t="s">
@@ -1295,7 +1294,7 @@
       <c r="I3" s="4">
         <v>2</v>
       </c>
-      <c r="J3" s="60"/>
+      <c r="J3" s="56"/>
       <c r="K3" t="s">
         <v>46</v>
       </c>
@@ -1317,7 +1316,7 @@
       <c r="S3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="T3" s="51">
+      <c r="T3" s="48">
         <v>44977</v>
       </c>
       <c r="U3" t="s">
@@ -1326,7 +1325,7 @@
       <c r="V3" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="W3" s="55" t="s">
+      <c r="W3" s="52" t="s">
         <v>123</v>
       </c>
       <c r="X3" t="s">
@@ -1340,7 +1339,7 @@
       <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="56" t="s">
         <v>127</v>
       </c>
       <c r="K4" t="s">
@@ -1368,7 +1367,7 @@
       <c r="S4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="T4" s="51">
+      <c r="T4" s="48">
         <v>44983</v>
       </c>
       <c r="U4" t="s">
@@ -1377,7 +1376,7 @@
       <c r="V4" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="W4" s="55" t="s">
+      <c r="W4" s="52" t="s">
         <v>123</v>
       </c>
       <c r="X4" t="s">
@@ -1409,7 +1408,7 @@
       <c r="I5" s="4">
         <v>4</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="56" t="s">
         <v>128</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1433,16 +1432,16 @@
       <c r="S5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="T5" s="51">
+      <c r="T5" s="48">
         <v>44986</v>
       </c>
-      <c r="U5" s="52">
+      <c r="U5" s="49">
         <v>45000</v>
       </c>
-      <c r="V5" s="53">
+      <c r="V5" s="50">
         <v>44993</v>
       </c>
-      <c r="W5" s="55">
+      <c r="W5" s="52">
         <v>0</v>
       </c>
       <c r="X5" t="s">
@@ -1477,7 +1476,7 @@
       <c r="I6" s="4">
         <v>5</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="56" t="s">
         <v>129</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -1503,16 +1502,16 @@
       <c r="S6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="T6" s="51">
+      <c r="T6" s="48">
         <v>45015</v>
       </c>
-      <c r="U6" s="52">
+      <c r="U6" s="49">
         <v>45024</v>
       </c>
-      <c r="V6" s="53">
+      <c r="V6" s="50">
         <v>45018</v>
       </c>
-      <c r="W6" s="56">
+      <c r="W6" s="52">
         <v>0</v>
       </c>
       <c r="X6" t="s">
@@ -1544,7 +1543,7 @@
       <c r="I7" s="4">
         <v>6</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="56" t="s">
         <v>130</v>
       </c>
       <c r="K7" t="s">
@@ -1558,7 +1557,7 @@
       </c>
       <c r="N7" s="4"/>
       <c r="O7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1572,7 +1571,7 @@
       <c r="S7" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T7" s="51">
+      <c r="T7" s="48">
         <v>44979</v>
       </c>
       <c r="U7" s="2" t="s">
@@ -1581,7 +1580,7 @@
       <c r="V7" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="W7" s="55" t="s">
+      <c r="W7" s="52" t="s">
         <v>123</v>
       </c>
       <c r="X7" t="s">
@@ -1616,12 +1615,12 @@
       <c r="I8" s="4">
         <v>7</v>
       </c>
-      <c r="J8" s="60"/>
+      <c r="J8" s="56"/>
       <c r="K8" t="s">
         <v>46</v>
       </c>
       <c r="N8" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -1638,7 +1637,7 @@
       <c r="S8" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T8" s="51">
+      <c r="T8" s="48">
         <v>44977</v>
       </c>
       <c r="U8" t="s">
@@ -1647,7 +1646,7 @@
       <c r="V8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="W8" s="55" t="s">
+      <c r="W8" s="52" t="s">
         <v>123</v>
       </c>
       <c r="X8" t="s">
@@ -1677,7 +1676,7 @@
       <c r="I9" s="4">
         <v>8</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="56" t="s">
         <v>126</v>
       </c>
       <c r="K9" t="s">
@@ -1691,7 +1690,7 @@
       </c>
       <c r="N9" s="4"/>
       <c r="O9">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1705,7 +1704,7 @@
       <c r="S9" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T9" s="51">
+      <c r="T9" s="48">
         <v>44983</v>
       </c>
       <c r="U9" t="s">
@@ -1714,7 +1713,7 @@
       <c r="V9" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="W9" s="55" t="s">
+      <c r="W9" s="52" t="s">
         <v>123</v>
       </c>
       <c r="X9" t="s">
@@ -1795,7 +1794,7 @@
       <c r="T11" s="6"/>
       <c r="U11" s="7"/>
       <c r="V11" s="9"/>
-      <c r="W11" s="57"/>
+      <c r="W11" s="53"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -1861,7 +1860,7 @@
       <c r="V13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W13" s="58"/>
+      <c r="W13" s="54"/>
       <c r="X13" s="27" t="s">
         <v>51</v>
       </c>
@@ -1912,7 +1911,7 @@
       <c r="V14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="W14" s="59"/>
+      <c r="W14" s="55"/>
       <c r="X14" s="29" t="s">
         <v>43</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>45</v>
       </c>
       <c r="V15" s="21"/>
-      <c r="W15" s="59"/>
+      <c r="W15" s="55"/>
       <c r="X15" s="29" t="s">
         <v>45</v>
       </c>
@@ -2181,7 +2180,7 @@
       </c>
     </row>
     <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="57" t="s">
         <v>114</v>
       </c>
       <c r="C28" s="1"/>
@@ -2207,7 +2206,7 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="49"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="44" t="s">
         <v>103</v>
       </c>
@@ -2223,7 +2222,7 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="49"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="4"/>
       <c r="D30" s="42"/>
       <c r="E30" t="s">
@@ -2244,7 +2243,7 @@
       </c>
     </row>
     <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="49"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="4"/>
       <c r="D31" s="43" t="s">
         <v>93</v>
@@ -2266,7 +2265,7 @@
       </c>
     </row>
     <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="49"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="4"/>
       <c r="G32" t="s">
         <v>45</v>
@@ -2276,7 +2275,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="49"/>
+      <c r="B33" s="58"/>
       <c r="C33" s="4"/>
       <c r="D33" s="41" t="s">
         <v>90</v>
@@ -2288,7 +2287,7 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="49"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="4"/>
       <c r="D34" s="42"/>
       <c r="E34" t="s">
@@ -2298,7 +2297,7 @@
       <c r="J34" s="5"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="49"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="4"/>
       <c r="D35" s="43" t="s">
         <v>93</v>
@@ -2310,12 +2309,12 @@
       <c r="J35" s="5"/>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="49"/>
+      <c r="B36" s="58"/>
       <c r="C36" s="4"/>
       <c r="J36" s="5"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="49"/>
+      <c r="B37" s="58"/>
       <c r="C37" s="44" t="s">
         <v>102</v>
       </c>
@@ -2334,7 +2333,7 @@
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="49"/>
+      <c r="B38" s="58"/>
       <c r="C38" s="46" t="s">
         <v>113</v>
       </c>
@@ -2359,17 +2358,17 @@
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="49"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="4"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="49"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="4"/>
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="49"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="44" t="s">
         <v>106</v>
       </c>
@@ -2379,7 +2378,7 @@
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="49"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="4"/>
       <c r="D42" t="s">
         <v>108</v>
@@ -2387,7 +2386,7 @@
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="49"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="4"/>
       <c r="D43" t="s">
         <v>109</v>
@@ -2395,7 +2394,7 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="49"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="4"/>
       <c r="D44" t="s">
         <v>110</v>
@@ -2403,12 +2402,12 @@
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="49"/>
+      <c r="B45" s="58"/>
       <c r="C45" s="4"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="50"/>
+      <c r="B46" s="59"/>
       <c r="C46" s="6" t="s">
         <v>112</v>
       </c>

</xml_diff>